<commit_message>
Random Forest grid param testing #4
</commit_message>
<xml_diff>
--- a/code/random_forest-outfiles/RFECV select 6 from 12/RFECV select 6 from 12.xlsx
+++ b/code/random_forest-outfiles/RFECV select 6 from 12/RFECV select 6 from 12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Research-Spring2021\code\random_forest-outfiles\RFECV select 6 from 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B9E50C-BF40-47E9-8046-145E85A3A3B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEDC874-09A2-429D-9D96-827AE4D991F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RFECV_RF_2021.04.29-13.30.08" sheetId="1" r:id="rId1"/>
@@ -1184,30 +1184,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$2:$AW$2</c:f>
+              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$15:$AW$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.71626598799999996</c:v>
+                  <c:v>0.71650400924999991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.709501669</c:v>
+                  <c:v>0.70947379474999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70571094499999998</c:v>
+                  <c:v>0.70575313891666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70220131299999999</c:v>
+                  <c:v>0.70218185716666659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69946177099999995</c:v>
+                  <c:v>0.69938973550000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69906862700000005</c:v>
+                  <c:v>0.69912160475000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.69801046</c:v>
+                  <c:v>0.69794408125000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,590 +1216,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$3:$AW$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71705442200000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70945389400000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70576007900000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70235833000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69955002399999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69905911799999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69789020700000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$4:$AW$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71624961300000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70945969399999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70575359999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70217728000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69963271199999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69914209900000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69793037999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$5:$AW$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71704782499999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.709498619</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70571065300000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70196493199999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69917547499999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69911562999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69794440599999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$6:$AW$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71703370700000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70945671099999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70580647100000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70218072099999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69953385700000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69914843699999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69797114900000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$7:$AW$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.716261123</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70946956900000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70576340999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.702208575</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.699135705</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69911503399999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69788518200000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$8:$AW$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71623924100000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70950267199999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70577503200000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70288655300000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.70007266000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69912594400000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69794706299999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$9:$AW$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71701662899999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70945076900000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70575701000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70214956399999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69919807700000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69915464199999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69792087599999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$10:$AW$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71624119799999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70951297499999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70574385799999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70174504599999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.699239214</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69914989400000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69796975900000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$11:$AW$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71622640599999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70946427000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70575306299999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.702336403</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69914048799999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69912329299999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.697936153</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$12:$AW$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71622890400000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70944754399999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.705763268</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70216141200000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69905185700000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69910377700000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69792065999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-9796-403B-93FA-3D4BD6C5278A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'RFECV_RF_2021.04.29-13.30.08'!$AQ$13:$AW$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.71618305500000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70946715100000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70574027800000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70181215699999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69948498599999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69915276199999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69800267999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-9796-403B-93FA-3D4BD6C5278A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3137,16 +2553,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3473,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AK10" sqref="AK10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5418,52 +4834,80 @@
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AE15">
-        <f>AVERAGE(AE2:AE13)</f>
+        <f t="shared" ref="AE15:AP15" si="0">AVERAGE(AE2:AE13)</f>
         <v>1</v>
       </c>
       <c r="AF15">
-        <f>AVERAGE(AF2:AF13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AG15">
-        <f>AVERAGE(AG2:AG13)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="AH15">
-        <f>AVERAGE(AH2:AH13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AI15">
-        <f>AVERAGE(AI2:AI13)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AJ15">
-        <f>AVERAGE(AJ2:AJ13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK15">
-        <f>AVERAGE(AK2:AK13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AL15">
-        <f>AVERAGE(AL2:AL13)</f>
+        <f t="shared" si="0"/>
         <v>4.083333333333333</v>
       </c>
       <c r="AM15">
-        <f>AVERAGE(AM2:AM13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AN15">
-        <f>AVERAGE(AN2:AN13)</f>
+        <f t="shared" si="0"/>
         <v>4.916666666666667</v>
       </c>
       <c r="AO15">
-        <f>AVERAGE(AO2:AO13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AP15">
-        <f>AVERAGE(AP2:AP13)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" ref="AQ15:AW15" si="1">AVERAGE(AQ2:AQ13)</f>
+        <v>0.71650400924999991</v>
+      </c>
+      <c r="AR15">
+        <f t="shared" si="1"/>
+        <v>0.70947379474999994</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="1"/>
+        <v>0.70575313891666669</v>
+      </c>
+      <c r="AT15">
+        <f t="shared" si="1"/>
+        <v>0.70218185716666659</v>
+      </c>
+      <c r="AU15">
+        <f t="shared" si="1"/>
+        <v>0.69938973550000005</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="1"/>
+        <v>0.69912160475000007</v>
+      </c>
+      <c r="AW15">
+        <f t="shared" si="1"/>
+        <v>0.69794408125000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>